<commit_message>
data enter as sample test
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -544,6 +544,28 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>pri</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ya</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Not Registered</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>